<commit_message>
fixed by 18466 ,问题清单
</commit_message>
<xml_diff>
--- a/core-db/src/main/java/com/hand/hls/中关村租赁核心业务系统框架升级项目_问题跟踪表_V2_20181113.xlsx
+++ b/core-db/src/main/java/com/hand/hls/中关村租赁核心业务系统框架升级项目_问题跟踪表_V2_20181113.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33824B70-6B4C-4E4F-BC4F-CF7343D47A35}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2138D942-B10A-473E-BC77-DCFA2FF6A0B6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7920" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,11 +49,11 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId34"/>
-    <pivotCache cacheId="6" r:id="rId35"/>
-    <pivotCache cacheId="7" r:id="rId36"/>
-    <pivotCache cacheId="8" r:id="rId37"/>
-    <pivotCache cacheId="9" r:id="rId38"/>
+    <pivotCache cacheId="0" r:id="rId34"/>
+    <pivotCache cacheId="1" r:id="rId35"/>
+    <pivotCache cacheId="2" r:id="rId36"/>
+    <pivotCache cacheId="3" r:id="rId37"/>
+    <pivotCache cacheId="4" r:id="rId38"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -19838,7 +19838,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000004000000}" name="数据透视表6" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000004000000}" name="数据透视表6" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="B34:C41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -20031,7 +20031,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="数据透视表3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="数据透视表3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="K4:L18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField dataField="1" showAll="0"/>
@@ -20168,7 +20168,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="数据透视表2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="数据透视表2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="B59:C66" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -20481,7 +20481,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="数据透视表1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="数据透视表1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
   <location ref="C5:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField dataField="1" showAll="0"/>
@@ -20651,7 +20651,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000003000000}" name="数据透视表4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000003000000}" name="数据透视表4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="K28:O58" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -23314,8 +23314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23539,7 +23539,7 @@
       <c r="N12" s="47"/>
       <c r="O12" s="47"/>
     </row>
-    <row r="13" spans="1:15" s="50" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A13" s="47">
         <v>2</v>
       </c>
@@ -23578,7 +23578,7 @@
       <c r="N13" s="47"/>
       <c r="O13" s="47"/>
     </row>
-    <row r="14" spans="1:15" s="50" customFormat="1" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="47">
         <v>3</v>
       </c>
@@ -24156,7 +24156,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="C29" s="53" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
fixed by 18466 ,bug fixed
</commit_message>
<xml_diff>
--- a/core-db/src/main/java/com/hand/hls/中关村租赁核心业务系统框架升级项目_问题跟踪表_V2_20181113.xlsx
+++ b/core-db/src/main/java/com/hand/hls/中关村租赁核心业务系统框架升级项目_问题跟踪表_V2_20181113.xlsx
@@ -3,22 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2138D942-B10A-473E-BC77-DCFA2FF6A0B6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750679E3-885C-4277-A442-C681ACEDDF27}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7920" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issue OverView" sheetId="5" state="hidden" r:id="rId1"/>
     <sheet name="问题图示" sheetId="4" state="hidden" r:id="rId2"/>
     <sheet name="Issue List" sheetId="1" r:id="rId3"/>
     <sheet name="LOOKUP" sheetId="7" state="hidden" r:id="rId4"/>
-    <sheet name="地区定义页面报错" sheetId="8" r:id="rId5"/>
-    <sheet name="PDF预览错误" sheetId="10" r:id="rId6"/>
+    <sheet name="地区定义页面报错" sheetId="8" state="hidden" r:id="rId5"/>
+    <sheet name="PDF预览错误" sheetId="10" state="hidden" r:id="rId6"/>
     <sheet name="立项新增按钮颜色" sheetId="11" state="hidden" r:id="rId7"/>
-    <sheet name="立项报告等按钮无颜色" sheetId="12" r:id="rId8"/>
+    <sheet name="立项报告等按钮无颜色" sheetId="12" state="hidden" r:id="rId8"/>
     <sheet name="合同文本生成格式有问题" sheetId="13" r:id="rId9"/>
-    <sheet name="标题不显示" sheetId="14" r:id="rId10"/>
-    <sheet name="数字溢出" sheetId="15" r:id="rId11"/>
+    <sheet name="标题不显示" sheetId="14" state="hidden" r:id="rId10"/>
+    <sheet name="数字溢出" sheetId="15" state="hidden" r:id="rId11"/>
     <sheet name="收款新增保存卡住" sheetId="16" r:id="rId12"/>
     <sheet name="按钮不整齐" sheetId="9" r:id="rId13"/>
     <sheet name="文字与按钮重叠" sheetId="18" r:id="rId14"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="208">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1350,7 +1350,97 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规_Sheet1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="67">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7349,13 +7439,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>665124</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>369849</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>132669</xdr:rowOff>
     </xdr:to>
@@ -7380,7 +7470,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="390525" y="0"/>
           <a:ext cx="13009524" cy="5447619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -19901,7 +19991,7 @@
     <dataField name="计数项:序号" fld="0" subtotal="count" baseField="12" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="36">
+    <format dxfId="48">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -20129,29 +20219,29 @@
     <dataField name="计数项:序号" fld="0" subtotal="count" baseField="7" baseItem="0"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="43">
+    <format dxfId="55">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="54">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="53">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="52">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -20420,7 +20510,7 @@
     <dataField name="计数项:序号" fld="0" subtotal="count" baseField="6" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="44">
+    <format dxfId="56">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -20569,16 +20659,16 @@
     <dataField name="计数项:序号" fld="0" subtotal="count" baseField="5" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="48">
+    <format dxfId="60">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="59">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -20882,19 +20972,19 @@
     <dataField name="计数项:序号" fld="0" subtotal="count" baseField="9" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="54">
+    <format dxfId="66">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="65">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="64">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="10" count="27">
@@ -20929,7 +21019,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -21340,7 +21430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
@@ -21354,8 +21444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21370,8 +21460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23314,8 +23404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23325,7 +23415,7 @@
     <col min="3" max="3" width="13.25" style="44" customWidth="1"/>
     <col min="4" max="4" width="12.875" style="44" customWidth="1"/>
     <col min="5" max="5" width="23.875" style="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.25" style="44" customWidth="1"/>
+    <col min="6" max="6" width="48.875" style="44" customWidth="1"/>
     <col min="7" max="7" width="9.125" style="44" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="44" customWidth="1"/>
     <col min="9" max="9" width="13.375" style="44" customWidth="1"/>
@@ -23539,7 +23629,7 @@
       <c r="N12" s="47"/>
       <c r="O12" s="47"/>
     </row>
-    <row r="13" spans="1:15" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" s="50" customFormat="1" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A13" s="47">
         <v>2</v>
       </c>
@@ -23578,7 +23668,7 @@
       <c r="N13" s="47"/>
       <c r="O13" s="47"/>
     </row>
-    <row r="14" spans="1:15" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" s="50" customFormat="1" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A14" s="47">
         <v>3</v>
       </c>
@@ -23651,9 +23741,6 @@
         <v>43418</v>
       </c>
       <c r="K15" s="49"/>
-      <c r="L15" s="47" t="s">
-        <v>204</v>
-      </c>
       <c r="M15" s="47"/>
       <c r="N15" s="47"/>
       <c r="O15" s="47"/>
@@ -23690,7 +23777,9 @@
         <v>43418</v>
       </c>
       <c r="K16" s="49"/>
-      <c r="L16" s="47"/>
+      <c r="L16" s="47" t="s">
+        <v>204</v>
+      </c>
       <c r="M16" s="47"/>
       <c r="N16" s="47"/>
       <c r="O16" s="47"/>
@@ -23700,7 +23789,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="C17" s="53" t="s">
         <v>33</v>
@@ -23727,7 +23816,9 @@
         <v>43418</v>
       </c>
       <c r="K17" s="49"/>
-      <c r="L17" s="47"/>
+      <c r="L17" s="47" t="s">
+        <v>202</v>
+      </c>
       <c r="M17" s="47"/>
       <c r="N17" s="47"/>
       <c r="O17" s="47"/>
@@ -23737,7 +23828,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="C18" s="53" t="s">
         <v>32</v>
@@ -23764,7 +23855,9 @@
         <v>43418</v>
       </c>
       <c r="K18" s="49"/>
-      <c r="L18" s="47"/>
+      <c r="L18" s="47" t="s">
+        <v>202</v>
+      </c>
       <c r="M18" s="47"/>
       <c r="N18" s="47"/>
       <c r="O18" s="47"/>
@@ -24188,7 +24281,7 @@
       <c r="N29" s="47"/>
       <c r="O29" s="47"/>
     </row>
-    <row r="30" spans="1:15" s="50" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" s="50" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="47">
         <v>19</v>
       </c>
@@ -25503,27 +25596,67 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A81:XFD1048576 A55:XFD78 G50:XFD54 A1:XFD12 A50:E54 A15:XFD18 O14:XFD14 A21:XFD21 A19:K20 M19:XFD20 A22:K22 M22:XFD22 A23:XFD49 A13:K14 M13:XFD13">
-    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
+  <conditionalFormatting sqref="A81:XFD1048576 A55:XFD78 G50:XFD54 A1:XFD12 A50:E54 O14:XFD14 A21:XFD21 A22:K22 M22:XFD22 A23:XFD49 M13:XFD13 A13:K15 M15:XFD15 A16:XFD16 A17:K20 M17:XFD20">
+    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
       <formula>"待确认"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
       <formula>"取消"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
       <formula>"已解决"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="58" operator="equal">
       <formula>"正在解决"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="60" operator="equal">
       <formula>"未处理"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="61" operator="equal">
       <formula>"未重现"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50:F53">
+    <cfRule type="cellIs" dxfId="41" priority="37" operator="equal">
+      <formula>"待确认"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
+      <formula>"取消"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+      <formula>"已解决"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+      <formula>"正在解决"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
+      <formula>"未处理"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
+      <formula>"未重现"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14:N14">
+    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
+      <formula>"待确认"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
+      <formula>"取消"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+      <formula>"已解决"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+      <formula>"正在解决"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+      <formula>"未处理"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+      <formula>"未重现"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:L20">
     <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"待确认"</formula>
     </cfRule>
@@ -25543,7 +25676,7 @@
       <formula>"未重现"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14:N14">
+  <conditionalFormatting sqref="L22">
     <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>"待确认"</formula>
     </cfRule>
@@ -25563,7 +25696,7 @@
       <formula>"未重现"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19:L20">
+  <conditionalFormatting sqref="L13">
     <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"待确认"</formula>
     </cfRule>
@@ -25583,7 +25716,7 @@
       <formula>"未重现"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22">
+  <conditionalFormatting sqref="L17">
     <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"待确认"</formula>
     </cfRule>
@@ -25603,7 +25736,7 @@
       <formula>"未重现"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
+  <conditionalFormatting sqref="L18">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"待确认"</formula>
     </cfRule>
@@ -25923,7 +26056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>

</xml_diff>